<commit_message>
101 Pass for KLIC
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{394E242C-43A5-4FF5-8B92-BE356AEAD4DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADA9B8AD-A9CA-47B9-BE1F-B525148DF62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=102</t>
+    <t>TestCaseNumber=101</t>
   </si>
   <si>
     <t>102</t>
@@ -616,7 +616,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Minor fix to TestRunner_KLI and better error reporting in ExcelReader
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADA9B8AD-A9CA-47B9-BE1F-B525148DF62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{ADA9B8AD-A9CA-47B9-BE1F-B525148DF62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F70E611-A683-4F98-936E-0AC83E3B5DCB}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -54,13 +54,13 @@
     <t>NumberOfBrowsers</t>
   </si>
   <si>
+    <t>http://kliappsvr:99/</t>
+  </si>
+  <si>
     <t>BaseURL</t>
   </si>
   <si>
     <t>https://uateinsurance.mykotaklife.com/einsurance</t>
-  </si>
-  <si>
-    <t>http://kliappsvr:99/</t>
   </si>
   <si>
     <t>TestCaseNumber</t>
@@ -538,19 +538,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -558,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -566,7 +567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -574,36 +575,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" s="7" t="s">
-        <v>8</v>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" tooltip="https://uateinsurance.mykotaklife.com/einsurance" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="https://uateinsurance.mykotaklife.com/einsurance" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B5" r:id="rId3" tooltip="https://uateinsurance.mykotaklife.com/einsurance" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -615,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
complete data for kli poc
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{ADA9B8AD-A9CA-47B9-BE1F-B525148DF62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F70E611-A683-4F98-936E-0AC83E3B5DCB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6852AC3B-1353-45EB-AED7-1A491CEF4475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>Properties</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>TestCaseNumber=101</t>
-  </si>
-  <si>
     <t>102</t>
   </si>
   <si>
@@ -94,13 +91,169 @@
   </si>
   <si>
     <t>105</t>
+  </si>
+  <si>
+    <t>1912</t>
+  </si>
+  <si>
+    <t>1913</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>1902</t>
+  </si>
+  <si>
+    <t>1903</t>
+  </si>
+  <si>
+    <t>1904</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>1906</t>
+  </si>
+  <si>
+    <t>1907</t>
+  </si>
+  <si>
+    <t>1908</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
+    <t>1910</t>
+  </si>
+  <si>
+    <t>1914</t>
+  </si>
+  <si>
+    <t>1915</t>
+  </si>
+  <si>
+    <t>1916</t>
+  </si>
+  <si>
+    <t>1917</t>
+  </si>
+  <si>
+    <t>1918</t>
+  </si>
+  <si>
+    <t>1919</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>1921</t>
+  </si>
+  <si>
+    <t>1922</t>
+  </si>
+  <si>
+    <t>1923</t>
+  </si>
+  <si>
+    <t>1924</t>
+  </si>
+  <si>
+    <t>1925</t>
+  </si>
+  <si>
+    <t>1926</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>TestCaseNumber=1911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +269,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -173,12 +332,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -194,6 +364,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,18 +719,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -567,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -575,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -586,7 +765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -610,20 +789,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -637,8 +816,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -648,12 +827,12 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -662,9 +841,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -673,9 +852,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -684,9 +863,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -695,7 +874,327 @@
         <v>15</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1898</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1899</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1900</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>1911</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for PDF Validations
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6852AC3B-1353-45EB-AED7-1A491CEF4475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63D756DB-44FE-4FCE-8309-7CDB9B088074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Properties</t>
   </si>
@@ -81,6 +81,9 @@
     <t>Smoke</t>
   </si>
   <si>
+    <t>TestCaseNumber=107</t>
+  </si>
+  <si>
     <t>102</t>
   </si>
   <si>
@@ -93,167 +96,167 @@
     <t>105</t>
   </si>
   <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1902</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1903</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1904</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1906</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1907</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1908</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1910</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>1912</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>1913</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
-    <t>1901</t>
-  </si>
-  <si>
-    <t>1902</t>
-  </si>
-  <si>
-    <t>1903</t>
-  </si>
-  <si>
-    <t>1904</t>
-  </si>
-  <si>
-    <t>1905</t>
-  </si>
-  <si>
-    <t>1906</t>
-  </si>
-  <si>
-    <t>1907</t>
-  </si>
-  <si>
-    <t>1908</t>
-  </si>
-  <si>
-    <t>1909</t>
-  </si>
-  <si>
-    <t>1910</t>
-  </si>
-  <si>
     <t>1914</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>1915</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>1916</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>1917</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>1918</t>
   </si>
   <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>1919</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>1920</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>1921</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>1922</t>
   </si>
   <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>1923</t>
   </si>
   <si>
+    <t>24</t>
+  </si>
+  <si>
     <t>1924</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
     <t>1925</t>
   </si>
   <si>
+    <t>26</t>
+  </si>
+  <si>
     <t>1926</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>27</t>
-  </si>
-  <si>
-    <t>TestCaseNumber=1911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,14 +726,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -746,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -754,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -765,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -789,20 +792,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -816,7 +819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="9">
         <v>101</v>
       </c>
@@ -827,12 +830,12 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -841,9 +844,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -852,9 +855,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -863,9 +866,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -874,9 +877,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>1898</v>
+    <row r="7" spans="1:4">
+      <c r="A7" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -885,9 +888,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1899</v>
+    <row r="8" spans="1:4">
+      <c r="A8" s="10">
+        <v>1898</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -896,9 +899,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -907,20 +910,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5">
+        <v>1900</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -929,267 +932,278 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8">
+        <v>1911</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>1911</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
framework can now read multiple pdf's in a single execution flow.
and updated data for klic poc
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B21F40-78B0-4EB1-88BD-9308C3B32B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AFA596-80BF-4733-9D9A-3179F50DD83E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="235">
   <si>
     <t>Properties</t>
   </si>
@@ -537,19 +537,205 @@
     <t>76</t>
   </si>
   <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>HHH</t>
-  </si>
-  <si>
     <t>http://kliappsitsvr/OnlineTermInsuranceNRI/</t>
   </si>
   <si>
-    <t>Nri</t>
-  </si>
-  <si>
-    <t>Groups=Smoke,Regression,Nri</t>
+    <t>TestCaseNumber=1974</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -1092,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,11 +1312,8 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,9 +1323,6 @@
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1151,9 +1331,6 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -1162,9 +1339,6 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1173,9 +1347,6 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1184,9 +1355,6 @@
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -1228,9 +1396,6 @@
       <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1239,9 +1404,6 @@
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1250,9 +1412,6 @@
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1261,9 +1420,6 @@
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1272,9 +1428,6 @@
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1283,745 +1436,821 @@
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>1911</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C37" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C38" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C39" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C42" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>80</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C45" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C46" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C48" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C49" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C50" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C51" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C53" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C54" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C55" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>91</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C57" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C58" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C59" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C60" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C61" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C62" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C63" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C65" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C66" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C68" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C69" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C70" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C71" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C72" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C74" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C76" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C77" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C78" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C79" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C81" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C82" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C83" t="s">
-        <v>168</v>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for Description in TestCase and Effective Report
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagasrinivast\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214D4881-24C8-46E1-9BAB-4E35E6CAA3A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A30C8-258D-422F-9068-D7C353249FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="356">
   <si>
     <t>Properties</t>
   </si>
@@ -744,7 +744,361 @@
     <t>Ec</t>
   </si>
   <si>
-    <t>Groups=Smoke,Nri,Ec</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Not a tobacco user, pg qualified and covered under kotak group insurance</t>
+  </si>
+  <si>
+    <t>TestDescription_1</t>
+  </si>
+  <si>
+    <t>TestDescription_2</t>
+  </si>
+  <si>
+    <t>TestDescription_10</t>
+  </si>
+  <si>
+    <t>TestDescription_11</t>
+  </si>
+  <si>
+    <t>TestDescription_12</t>
+  </si>
+  <si>
+    <t>TestDescription_13</t>
+  </si>
+  <si>
+    <t>TestDescription_3</t>
+  </si>
+  <si>
+    <t>TestDescription_4</t>
+  </si>
+  <si>
+    <t>TestDescription_5</t>
+  </si>
+  <si>
+    <t>TestDescription_6</t>
+  </si>
+  <si>
+    <t>TestDescription_7</t>
+  </si>
+  <si>
+    <t>TestDescription_8</t>
+  </si>
+  <si>
+    <t>TestDescription_9</t>
+  </si>
+  <si>
+    <t>TestDescription_14</t>
+  </si>
+  <si>
+    <t>TestDescription_15</t>
+  </si>
+  <si>
+    <t>TestDescription_16</t>
+  </si>
+  <si>
+    <t>TestDescription_17</t>
+  </si>
+  <si>
+    <t>TestDescription_18</t>
+  </si>
+  <si>
+    <t>TestDescription_19</t>
+  </si>
+  <si>
+    <t>TestDescription_20</t>
+  </si>
+  <si>
+    <t>TestDescription_21</t>
+  </si>
+  <si>
+    <t>TestDescription_22</t>
+  </si>
+  <si>
+    <t>TestDescription_23</t>
+  </si>
+  <si>
+    <t>TestDescription_24</t>
+  </si>
+  <si>
+    <t>TestDescription_25</t>
+  </si>
+  <si>
+    <t>TestDescription_26</t>
+  </si>
+  <si>
+    <t>TestDescription_27</t>
+  </si>
+  <si>
+    <t>TestDescription_28</t>
+  </si>
+  <si>
+    <t>TestDescription_29</t>
+  </si>
+  <si>
+    <t>TestDescription_30</t>
+  </si>
+  <si>
+    <t>TestDescription_31</t>
+  </si>
+  <si>
+    <t>TestDescription_32</t>
+  </si>
+  <si>
+    <t>TestDescription_33</t>
+  </si>
+  <si>
+    <t>TestDescription_34</t>
+  </si>
+  <si>
+    <t>TestDescription_35</t>
+  </si>
+  <si>
+    <t>TestDescription_36</t>
+  </si>
+  <si>
+    <t>TestDescription_37</t>
+  </si>
+  <si>
+    <t>TestDescription_38</t>
+  </si>
+  <si>
+    <t>TestDescription_39</t>
+  </si>
+  <si>
+    <t>TestDescription_40</t>
+  </si>
+  <si>
+    <t>TestDescription_41</t>
+  </si>
+  <si>
+    <t>TestDescription_42</t>
+  </si>
+  <si>
+    <t>TestDescription_43</t>
+  </si>
+  <si>
+    <t>TestDescription_44</t>
+  </si>
+  <si>
+    <t>TestDescription_45</t>
+  </si>
+  <si>
+    <t>TestDescription_46</t>
+  </si>
+  <si>
+    <t>TestDescription_47</t>
+  </si>
+  <si>
+    <t>TestDescription_48</t>
+  </si>
+  <si>
+    <t>TestDescription_49</t>
+  </si>
+  <si>
+    <t>TestDescription_50</t>
+  </si>
+  <si>
+    <t>TestDescription_51</t>
+  </si>
+  <si>
+    <t>TestDescription_52</t>
+  </si>
+  <si>
+    <t>TestDescription_53</t>
+  </si>
+  <si>
+    <t>TestDescription_54</t>
+  </si>
+  <si>
+    <t>TestDescription_55</t>
+  </si>
+  <si>
+    <t>TestDescription_56</t>
+  </si>
+  <si>
+    <t>TestDescription_57</t>
+  </si>
+  <si>
+    <t>TestDescription_58</t>
+  </si>
+  <si>
+    <t>TestDescription_59</t>
+  </si>
+  <si>
+    <t>TestDescription_60</t>
+  </si>
+  <si>
+    <t>TestDescription_61</t>
+  </si>
+  <si>
+    <t>TestDescription_62</t>
+  </si>
+  <si>
+    <t>TestDescription_63</t>
+  </si>
+  <si>
+    <t>TestDescription_64</t>
+  </si>
+  <si>
+    <t>TestDescription_65</t>
+  </si>
+  <si>
+    <t>TestDescription_66</t>
+  </si>
+  <si>
+    <t>TestDescription_67</t>
+  </si>
+  <si>
+    <t>TestDescription_68</t>
+  </si>
+  <si>
+    <t>TestDescription_69</t>
+  </si>
+  <si>
+    <t>TestDescription_70</t>
+  </si>
+  <si>
+    <t>TestDescription_71</t>
+  </si>
+  <si>
+    <t>TestDescription_72</t>
+  </si>
+  <si>
+    <t>TestDescription_73</t>
+  </si>
+  <si>
+    <t>TestDescription_74</t>
+  </si>
+  <si>
+    <t>TestDescription_75</t>
+  </si>
+  <si>
+    <t>TestDescription_76</t>
+  </si>
+  <si>
+    <t>TestDescription_77</t>
+  </si>
+  <si>
+    <t>TestDescription_78</t>
+  </si>
+  <si>
+    <t>TestDescription_79</t>
+  </si>
+  <si>
+    <t>TestDescription_80</t>
+  </si>
+  <si>
+    <t>TestDescription_81</t>
+  </si>
+  <si>
+    <t>TestDescription_82</t>
+  </si>
+  <si>
+    <t>TestDescription_83</t>
+  </si>
+  <si>
+    <t>TestDescription_84</t>
+  </si>
+  <si>
+    <t>TestDescription_85</t>
+  </si>
+  <si>
+    <t>TestDescription_86</t>
+  </si>
+  <si>
+    <t>TestDescription_87</t>
+  </si>
+  <si>
+    <t>TestDescription_88</t>
+  </si>
+  <si>
+    <t>TestDescription_89</t>
+  </si>
+  <si>
+    <t>TestDescription_90</t>
+  </si>
+  <si>
+    <t>TestDescription_91</t>
+  </si>
+  <si>
+    <t>TestDescription_92</t>
+  </si>
+  <si>
+    <t>TestDescription_93</t>
+  </si>
+  <si>
+    <t>TestDescription_94</t>
+  </si>
+  <si>
+    <t>TestDescription_95</t>
+  </si>
+  <si>
+    <t>TestDescription_96</t>
+  </si>
+  <si>
+    <t>TestDescription_97</t>
+  </si>
+  <si>
+    <t>TestDescription_98</t>
+  </si>
+  <si>
+    <t>TestDescription_99</t>
+  </si>
+  <si>
+    <t>TestDescription_100</t>
+  </si>
+  <si>
+    <t>TestDescription_101</t>
+  </si>
+  <si>
+    <t>TestDescription_102</t>
+  </si>
+  <si>
+    <t>TestDescription_103</t>
+  </si>
+  <si>
+    <t>TestDescription_104</t>
+  </si>
+  <si>
+    <t>TestDescription_105</t>
+  </si>
+  <si>
+    <t>TestDescription_106</t>
+  </si>
+  <si>
+    <t>TestDescription_107</t>
+  </si>
+  <si>
+    <t>TestDescription_108</t>
+  </si>
+  <si>
+    <t>TestDescription_109</t>
+  </si>
+  <si>
+    <t>TestDescription_110</t>
+  </si>
+  <si>
+    <t>TestDescription_111</t>
+  </si>
+  <si>
+    <t>TestDescription_112</t>
+  </si>
+  <si>
+    <t>TestDescription_113</t>
+  </si>
+  <si>
+    <t>TestDescription_114</t>
+  </si>
+  <si>
+    <t>TestDescription_115</t>
+  </si>
+  <si>
+    <t>TestDescription_116</t>
+  </si>
+  <si>
+    <t>Groups=kjh,Smoke,Nri,Ec</t>
   </si>
 </sst>
 </file>
@@ -1287,1320 +1641,1674 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="1" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>101</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>235</v>
       </c>
-      <c r="D2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1898</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1899</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1900</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>1911</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C53" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C54" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C58" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C59" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C84" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C85" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C86" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C87" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C88" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C89" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C90" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C91" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C92" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C93" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C94" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C95" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C96" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C97" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C98" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C99" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C100" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C101" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C102" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C103" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C104" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C105" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C106" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C107" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C108" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C109" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C110" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C111" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C112" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C113" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C114" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C115" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C116" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C117" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
latest data for KLIC POC
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagasrinivast\git\VMSeleniumFramework\resources\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A30C8-258D-422F-9068-D7C353249FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A71E1C-B6AC-4BE1-B45E-DC525C75F005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="362">
   <si>
     <t>Properties</t>
   </si>
@@ -1098,7 +1098,25 @@
     <t>TestDescription_116</t>
   </si>
   <si>
-    <t>Groups=kjh,Smoke,Nri,Ec</t>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>TestDescription_117</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>TPI</t>
+  </si>
+  <si>
+    <t>https://uateinsurance.mykotaklife.com/einsurance/Aggregator.html</t>
+  </si>
+  <si>
+    <t>http://kliappsitsvr/OnlineTermInsurance/</t>
+  </si>
+  <si>
+    <t>TestCaseNumber=1936</t>
   </si>
 </sst>
 </file>
@@ -1569,17 +1587,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1621,37 +1639,55 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>168</v>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" tooltip="https://uateinsurance.mykotaklife.com/einsurance" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{6720A39D-390C-4283-B2A7-C4B04C8B18C8}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{22324165-6189-4DFD-A84C-654307E2A730}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{8833356A-A9AA-4295-81FA-CD936ACCC769}"/>
+    <hyperlink ref="B5" r:id="rId5" tooltip="https://uateinsurance.mykotaklife.com/einsurance" xr:uid="{31B31E5C-5764-4F45-B024-433B9BA006F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="21.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,8 +1720,8 @@
       <c r="D2" t="s">
         <v>235</v>
       </c>
-      <c r="E2" t="s">
-        <v>355</v>
+      <c r="E2" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,6 +1737,7 @@
       <c r="D3" t="s">
         <v>235</v>
       </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -3310,6 +3347,20 @@
       </c>
       <c r="D118" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D119" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated NRI test data
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\CodeLessFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0244770E-925D-4A0D-80A1-A216932ABB6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08F6CEC-7855-432A-9844-E0F7C09398BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1791,7 +1791,7 @@
     <t>TestCaseNumber=1912,1909,1920,1898,1918,1919,1906,1903,1902,1901,1900,1922</t>
   </si>
   <si>
-    <t>TestCaseNumber=1910</t>
+    <t>Groups=Nri</t>
   </si>
 </sst>
 </file>
@@ -2419,8 +2419,8 @@
   <dimension ref="A1:E297"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,7 +2462,7 @@
       <c r="D2" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>586</v>
       </c>
     </row>

</xml_diff>

<commit_message>
case - text area included
</commit_message>
<xml_diff>
--- a/resources/test_data/TestRunner_KLI.xlsx
+++ b/resources/test_data/TestRunner_KLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\CodeLessFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08F6CEC-7855-432A-9844-E0F7C09398BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9AF156-ECE5-4AD9-83C8-559055875EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="607">
   <si>
     <t>Properties</t>
   </si>
@@ -1788,10 +1788,70 @@
     <t>aasASAF</t>
   </si>
   <si>
-    <t>TestCaseNumber=1912,1909,1920,1898,1918,1919,1906,1903,1902,1901,1900,1922</t>
-  </si>
-  <si>
-    <t>Groups=Nri</t>
+    <t>5012</t>
+  </si>
+  <si>
+    <t>5013</t>
+  </si>
+  <si>
+    <t>5014</t>
+  </si>
+  <si>
+    <t>5015</t>
+  </si>
+  <si>
+    <t>5016</t>
+  </si>
+  <si>
+    <t>5017</t>
+  </si>
+  <si>
+    <t>5018</t>
+  </si>
+  <si>
+    <t>5019</t>
+  </si>
+  <si>
+    <t>5020</t>
+  </si>
+  <si>
+    <t>Sprint4</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_01</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_02</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_03</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_04</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_05</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_06</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_07</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_08</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_09</t>
+  </si>
+  <si>
+    <t>Sprint4_Tc_10</t>
+  </si>
+  <si>
+    <t>5021</t>
+  </si>
+  <si>
+    <t>TestCaseNumber=5013</t>
   </si>
 </sst>
 </file>
@@ -1922,7 +1982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1960,6 +2020,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2416,11 +2479,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E297"/>
+  <dimension ref="A1:E307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,8 +2525,8 @@
       <c r="D2" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>586</v>
+      <c r="E2" s="13" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,9 +2574,7 @@
       <c r="D5" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>585</v>
-      </c>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -6633,6 +6694,146 @@
         <v>141</v>
       </c>
       <c r="D297" s="9"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>594</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>